<commit_message>
fix & update v.2.0
</commit_message>
<xml_diff>
--- a/Register.xlsx
+++ b/Register.xlsx
@@ -1,61 +1,144 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jowita\OneDrive\Pulpit\STUDIA\SEM_21L\PIU\PIKOPIU\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jowita\OneDrive\Pulpit\register panel jfx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35EA81B0-6B32-4071-BDD9-0228ACD7A03A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DCB7F37-044A-432E-A28F-74D8428580AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="576" windowWidth="11520" windowHeight="9264" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4032" yWindow="708" windowWidth="16296" windowHeight="9264" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Rejestr użytkowników" sheetId="1" r:id="rId1"/>
+    <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Surname</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>Date of birth</t>
-  </si>
-  <si>
-    <t>Sex</t>
-  </si>
-  <si>
-    <t>User Register</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+  <si>
+    <t>USER PERSONAL DATA</t>
+  </si>
+  <si>
+    <t>USERNAME</t>
+  </si>
+  <si>
+    <t>NAME</t>
+  </si>
+  <si>
+    <t>SURNAME</t>
+  </si>
+  <si>
+    <t>EMAIL</t>
+  </si>
+  <si>
+    <t>PASSWORD</t>
+  </si>
+  <si>
+    <t>DATE-OF-BIRTH</t>
+  </si>
+  <si>
+    <t>SEX</t>
+  </si>
+  <si>
+    <t>jankowalski96</t>
+  </si>
+  <si>
+    <t>Jan</t>
+  </si>
+  <si>
+    <t>Kowalski</t>
+  </si>
+  <si>
+    <t>jankowalski@wp.pl</t>
+  </si>
+  <si>
+    <t>2022-07-09</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>britneYy</t>
+  </si>
+  <si>
+    <t>Britney</t>
+  </si>
+  <si>
+    <t>Spears</t>
+  </si>
+  <si>
+    <t>britneybeach@gmail.com</t>
+  </si>
+  <si>
+    <t>1234566</t>
+  </si>
+  <si>
+    <t>2022-07-04</t>
+  </si>
+  <si>
+    <t>female</t>
+  </si>
+  <si>
+    <t>lordvador</t>
+  </si>
+  <si>
+    <t>Sam</t>
+  </si>
+  <si>
+    <t>Vador</t>
+  </si>
+  <si>
+    <t>sunsamvador@gmail.com</t>
+  </si>
+  <si>
+    <t>sumvadi</t>
+  </si>
+  <si>
+    <t>2022-07-28</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color indexed="8"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -68,12 +151,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF66FF"/>
+        <fgColor rgb="FFFF99FF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -82,78 +165,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -162,31 +183,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -197,6 +199,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF99FF"/>
       <color rgb="FFFF66FF"/>
     </mruColors>
   </colors>
@@ -508,24 +511,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="G5" sqref="A5:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="28.44140625" customWidth="1"/>
-    <col min="6" max="6" width="15.77734375" customWidth="1"/>
-    <col min="8" max="8" width="7.5546875" customWidth="1"/>
-    <col min="9" max="9" width="8.88671875" hidden="1" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="11.6640625"/>
+    <col min="2" max="2" customWidth="true" width="11.21875"/>
+    <col min="3" max="3" customWidth="true" width="12.0"/>
+    <col min="4" max="4" customWidth="true" width="26.5546875"/>
+    <col min="5" max="5" customWidth="true" width="13.77734375"/>
+    <col min="6" max="6" customWidth="true" width="16.33203125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -533,62 +537,104 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="F2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="6"/>
-      <c r="I2" s="7"/>
+      <c r="G2" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="9"/>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:I3"/>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>